<commit_message>
updated performance test swetha excel
</commit_message>
<xml_diff>
--- a/MMS/Test Cases/Monitor app/Performance tests-swetha.xlsx
+++ b/MMS/Test Cases/Monitor app/Performance tests-swetha.xlsx
@@ -2707,8 +2707,8 @@
   <dimension ref="A2:I76"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F37" sqref="F37"/>
+      <pane ySplit="2" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
updatemonitor ap test case performance test swetha
</commit_message>
<xml_diff>
--- a/MMS/Test Cases/Monitor app/Performance tests-swetha.xlsx
+++ b/MMS/Test Cases/Monitor app/Performance tests-swetha.xlsx
@@ -82,7 +82,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F43" authorId="0">
+    <comment ref="F44" authorId="0">
       <text>
         <r>
           <rPr>
@@ -111,7 +111,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="221">
   <si>
     <t>time for upload</t>
   </si>
@@ -948,6 +948,23 @@
   </si>
   <si>
     <t>Actual Result</t>
+  </si>
+  <si>
+    <t>Share a Qrcode and scan</t>
+  </si>
+  <si>
+    <t>1. Choose place media as the category
+2. Capture an image and save
+3.  Select QR code to 'Identify media to link' 
+4. The barcode scanner opens.
+5. Select the share option in the scanner
+6. Enter a QRcode value
+7. Share the Qrcode image that gets generated (watsap, mail etc)
+8. scan the shared QRcode</t>
+  </si>
+  <si>
+    <t>1. If it is a valid QR code, the linked media must be retirved and displayed in link monitor.
+2. If the selected value of qrcode is not linked to any media, then the app must display a message 'The qrcode is not linked to any media. You want to link itnow.....'</t>
   </si>
 </sst>
 </file>
@@ -2704,11 +2721,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:I76"/>
+  <dimension ref="A2:I77"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D30" sqref="D30"/>
+      <pane ySplit="2" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F78" sqref="F78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3106,49 +3123,49 @@
         <v>213</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="90" x14ac:dyDescent="0.25">
-      <c r="A29" s="16">
+    <row r="29" spans="1:6" ht="135" x14ac:dyDescent="0.25">
+      <c r="A29" s="16"/>
+      <c r="C29" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="D29" s="17" t="s">
+        <v>219</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="A30" s="16">
         <v>26</v>
       </c>
-      <c r="C29" s="2" t="s">
+      <c r="C30" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="D29" s="17" t="s">
+      <c r="D30" s="17" t="s">
         <v>215</v>
       </c>
-      <c r="F29" s="2" t="s">
+      <c r="F30" s="2" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="16">
+    <row r="31" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" s="16">
         <v>27</v>
       </c>
-      <c r="D30" s="2" t="s">
+      <c r="D31" s="2" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A31" s="16">
+    <row r="32" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A32" s="16">
         <v>28</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="C32" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="D31" s="2" t="s">
+      <c r="D32" s="2" t="s">
         <v>184</v>
-      </c>
-      <c r="F31" s="20" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A32" s="16"/>
-      <c r="C32" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>183</v>
       </c>
       <c r="F32" s="20" t="s">
         <v>182</v>
@@ -3157,443 +3174,455 @@
     <row r="33" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A33" s="16"/>
       <c r="C33" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="F33" s="20" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A34" s="16">
-        <v>29</v>
-      </c>
+      <c r="A34" s="16"/>
       <c r="C34" s="2" t="s">
-        <v>88</v>
+        <v>187</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="F34" s="20" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A35" s="16">
+        <v>29</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="F35" s="20" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="A36" s="16">
         <v>30</v>
       </c>
-      <c r="C35" s="2" t="s">
+      <c r="C36" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D35" s="17" t="s">
+      <c r="D36" s="17" t="s">
         <v>190</v>
       </c>
-      <c r="F35" s="2" t="s">
+      <c r="F36" s="2" t="s">
         <v>191</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="16">
-        <v>31</v>
-      </c>
-      <c r="D36" s="4" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="16">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F37" s="2" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="16">
+        <v>32</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="16">
         <v>33</v>
       </c>
-      <c r="D38" s="4" t="s">
+      <c r="D39" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="F38" s="2" t="s">
+      <c r="F39" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A39" s="16">
+    <row r="40" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A40" s="16">
         <v>34</v>
       </c>
-      <c r="D39" s="2" t="s">
+      <c r="D40" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="F39" s="2"/>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="16">
-        <v>35</v>
-      </c>
-      <c r="D40" s="4" t="s">
-        <v>10</v>
       </c>
       <c r="F40" s="2"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="16">
+        <v>35</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F41" s="2"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="16">
         <v>36</v>
       </c>
-      <c r="D41" s="4" t="s">
+      <c r="D42" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="F41" s="2"/>
-    </row>
-    <row r="42" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A42" s="16">
+      <c r="F42" s="2"/>
+    </row>
+    <row r="43" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A43" s="16">
         <v>37</v>
       </c>
-      <c r="C42" s="4" t="s">
+      <c r="C43" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D42" s="2" t="s">
+      <c r="D43" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="F42" s="2" t="s">
+      <c r="F43" s="2" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A43" s="16"/>
-      <c r="C43" s="2" t="s">
+    <row r="44" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A44" s="16"/>
+      <c r="C44" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="D43" s="2" t="s">
+      <c r="D44" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="F43" s="2" t="s">
+      <c r="F44" s="2" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A44" s="16">
-        <v>38</v>
-      </c>
-      <c r="C44" s="2"/>
-      <c r="D44" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="E44" s="2"/>
     </row>
     <row r="45" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A45" s="16">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C45" s="2"/>
       <c r="D45" s="2" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="E45" s="2"/>
     </row>
-    <row r="46" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A46" s="16">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C46" s="2"/>
       <c r="D46" s="2" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="E46" s="2"/>
     </row>
     <row r="47" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="16">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C47" s="2"/>
       <c r="D47" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E47" s="2"/>
     </row>
     <row r="48" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" s="16">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C48" s="2"/>
       <c r="D48" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="E48" s="2"/>
+    </row>
+    <row r="49" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A49" s="16">
+        <v>42</v>
+      </c>
+      <c r="C49" s="2"/>
+      <c r="D49" s="2" t="s">
         <v>94</v>
-      </c>
-      <c r="E48" s="2"/>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="16">
-        <v>43</v>
-      </c>
-      <c r="D49" s="2" t="s">
-        <v>96</v>
       </c>
       <c r="E49" s="2"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="16">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
       <c r="E50" s="2"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="16">
-        <v>45</v>
-      </c>
-      <c r="D51" s="4" t="s">
-        <v>9</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E51" s="2"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="16">
+        <v>45</v>
+      </c>
+      <c r="D52" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" s="16">
         <v>46</v>
       </c>
-      <c r="D52" s="4" t="s">
+      <c r="D53" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="53" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A53" s="16">
+    <row r="54" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A54" s="16">
         <v>47</v>
       </c>
-      <c r="C53" s="2" t="s">
+      <c r="C54" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D53" s="2" t="s">
+      <c r="D54" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="F53" s="2" t="s">
+      <c r="F54" s="2" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="54" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A54" s="16">
+    <row r="55" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A55" s="16">
         <v>51</v>
       </c>
-      <c r="D54" s="2" t="s">
+      <c r="D55" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="E54" s="2"/>
-      <c r="F54" s="2" t="s">
+      <c r="E55" s="2"/>
+      <c r="F55" s="2" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="55" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A55" s="16">
+    <row r="56" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A56" s="16">
         <v>52</v>
       </c>
-      <c r="D55" s="2" t="s">
+      <c r="D56" s="2" t="s">
         <v>86</v>
-      </c>
-      <c r="E55" s="2"/>
-      <c r="F55" s="2"/>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" s="16">
-        <v>53</v>
-      </c>
-      <c r="D56" s="2" t="s">
-        <v>89</v>
       </c>
       <c r="E56" s="2"/>
       <c r="F56" s="2"/>
     </row>
-    <row r="57" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="16">
+        <v>53</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="E57" s="2"/>
+      <c r="F57" s="2"/>
+    </row>
+    <row r="58" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A58" s="16">
         <v>54</v>
       </c>
-      <c r="D57" s="2" t="s">
+      <c r="D58" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="F57" s="2"/>
-    </row>
-    <row r="58" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A58" s="16">
+      <c r="F58" s="2"/>
+    </row>
+    <row r="59" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A59" s="16">
         <v>55</v>
       </c>
-      <c r="D58" s="2" t="s">
+      <c r="D59" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="E58" s="2"/>
-      <c r="F58" s="2"/>
-    </row>
-    <row r="59" spans="1:6" ht="135" x14ac:dyDescent="0.25">
-      <c r="A59" s="16">
+      <c r="E59" s="2"/>
+      <c r="F59" s="2"/>
+    </row>
+    <row r="60" spans="1:6" ht="135" x14ac:dyDescent="0.25">
+      <c r="A60" s="16">
         <v>56</v>
       </c>
-      <c r="C59" s="2" t="s">
+      <c r="C60" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="D59" s="2" t="s">
+      <c r="D60" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="E59" s="2"/>
-      <c r="F59" s="2" t="s">
+      <c r="E60" s="2"/>
+      <c r="F60" s="2" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="16"/>
-      <c r="C60" s="2"/>
-      <c r="D60" s="2"/>
-      <c r="E60" s="2"/>
-      <c r="F60" s="2"/>
-    </row>
-    <row r="61" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A61" s="16">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" s="16"/>
+      <c r="C61" s="2"/>
+      <c r="D61" s="2"/>
+      <c r="E61" s="2"/>
+      <c r="F61" s="2"/>
+    </row>
+    <row r="62" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A62" s="16">
         <v>57</v>
       </c>
-      <c r="D61" s="2" t="s">
+      <c r="D62" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="E61" s="2"/>
-    </row>
-    <row r="62" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A62" s="16">
+      <c r="E62" s="2"/>
+    </row>
+    <row r="63" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A63" s="16">
         <v>58</v>
       </c>
-      <c r="D62" s="2" t="s">
+      <c r="D63" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="E62" s="2"/>
-      <c r="F62" s="2" t="s">
+      <c r="E63" s="2"/>
+      <c r="F63" s="2" t="s">
         <v>102</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A63" s="16">
-        <v>59</v>
-      </c>
-      <c r="D63" s="2" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="64" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A64" s="16">
+        <v>59</v>
+      </c>
+      <c r="D64" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A65" s="16">
         <v>60</v>
       </c>
-      <c r="D64" s="2" t="s">
+      <c r="D65" s="2" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A65" s="16">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" s="16">
         <v>61</v>
       </c>
-      <c r="D65" s="4" t="s">
+      <c r="D66" s="4" t="s">
         <v>105</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A66" s="16">
-        <v>62</v>
-      </c>
-      <c r="D66" s="2" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="67" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A67" s="16">
+        <v>62</v>
+      </c>
+      <c r="D67" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A68" s="16">
         <v>63</v>
       </c>
-      <c r="D67" s="2" t="s">
+      <c r="D68" s="2" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A68" s="16">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" s="16">
         <v>64</v>
       </c>
-      <c r="D68" s="4" t="s">
+      <c r="D69" s="4" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="69" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A69" s="16">
-        <v>65</v>
-      </c>
-      <c r="D69" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="E69" s="2"/>
     </row>
     <row r="70" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A70" s="16">
+        <v>65</v>
+      </c>
+      <c r="D70" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="E70" s="2"/>
+    </row>
+    <row r="71" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A71" s="16">
         <v>66</v>
       </c>
-      <c r="D70" s="2" t="s">
+      <c r="D71" s="2" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="71" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A71" s="16">
+    <row r="72" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A72" s="16">
         <v>67</v>
       </c>
-      <c r="D71" s="2" t="s">
+      <c r="D72" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="E71" s="2"/>
-    </row>
-    <row r="72" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A72" s="16">
+      <c r="E72" s="2"/>
+    </row>
+    <row r="73" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A73" s="16">
         <v>68</v>
-      </c>
-      <c r="C72" s="2"/>
-      <c r="D72" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="E72" s="2"/>
-    </row>
-    <row r="73" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A73" s="16">
-        <v>69</v>
       </c>
       <c r="C73" s="2"/>
       <c r="D73" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="E73" s="2"/>
+    </row>
+    <row r="74" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A74" s="16">
+        <v>69</v>
+      </c>
+      <c r="C74" s="2"/>
+      <c r="D74" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="E73" s="2"/>
-    </row>
-    <row r="74" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A74" s="16">
+      <c r="E74" s="2"/>
+    </row>
+    <row r="75" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A75" s="16">
         <v>70</v>
       </c>
-      <c r="C74" s="2" t="s">
+      <c r="C75" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="D74" s="4" t="s">
+      <c r="D75" s="4" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="75" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A75" s="16">
+    <row r="76" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A76" s="16">
         <v>71</v>
       </c>
-      <c r="C75" s="2" t="s">
+      <c r="C76" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="D75" s="4" t="s">
+      <c r="D76" s="4" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A76" s="16">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77" s="16">
         <v>72</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A2:I2"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G8:G65">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G8:G66">
       <formula1>"Pass, Fail, clarification"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>